<commit_message>
ServiceLevel translations will stored in AppTranslations.
</commit_message>
<xml_diff>
--- a/app/Services/DataLoader/Importers/OemsImporterTest.xlsx
+++ b/app/Services/DataLoader/Importers/OemsImporterTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t xml:space="preserve">Vendor</t>
   </si>
@@ -99,10 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve">Level LC French</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LC Description French
-line of text</t>
   </si>
   <si>
     <t xml:space="preserve">Level LC</t>
@@ -207,13 +203,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -244,17 +244,17 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.78"/>
   </cols>
   <sheetData>
@@ -284,49 +284,49 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -338,65 +338,63 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="3" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
`TextNormalizer` and `StringNormalizer` will remove NBSP characters.
</commit_message>
<xml_diff>
--- a/app/Services/DataLoader/Importers/OemsImporterTest.xlsx
+++ b/app/Services/DataLoader/Importers/OemsImporterTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t xml:space="preserve">Vendor</t>
   </si>
@@ -59,73 +59,80 @@
 line of text</t>
   </si>
   <si>
+    <t xml:space="preserve">Level LA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LA Description
+line of text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LB French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LB Description French
+line of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LB Description
+line of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LC French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LC Description
+line of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LD French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LD Description French
+line of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level LD Description
+line of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level LA</t>
   </si>
   <si>
     <t xml:space="preserve">Level LA Description
 line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LB French</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LB Description French
-line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LB Description
-line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LC French</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LC Description
-line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LD French</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LD Description French
-line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level LD Description
-line of text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBA</t>
   </si>
 </sst>
 </file>
@@ -244,10 +251,10 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.95"/>
@@ -392,10 +399,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>